<commit_message>
Usman - new user added to Cobal Users
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C766944
</commit_message>
<xml_diff>
--- a/PPIUK-Should/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Should/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="146">
   <si>
     <t>UserName</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>anztestuser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>Linking_AutoUser</t>
+  </si>
+  <si>
+    <t>Default user for Linking tests</t>
+  </si>
+  <si>
+    <t>linking.autouser@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -846,9 +855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1871,6 +1882,25 @@
       </c>
       <c r="G51" s="6" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>